<commit_message>
Added new method and tests for BigIntFixedDecimal{}.SetNumStr().
</commit_message>
<xml_diff>
--- a/notes/logarithms/logcalcs.xlsx
+++ b/notes/logarithms/logcalcs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gowork\src\MikeAustin71\mathopsgo\notes\logarithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2CC054A-F6BA-4A47-9F45-79BC9749673C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E78188C7-B094-4965-937F-5740FB61D4A1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26445" windowHeight="4560" activeTab="6" xr2:uid="{118135A5-616A-4318-8E98-F148E833D54E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26445" windowHeight="4560" activeTab="7" xr2:uid="{118135A5-616A-4318-8E98-F148E833D54E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,8 @@
     <sheet name="TableTest" sheetId="5" r:id="rId5"/>
     <sheet name="TableTest2" sheetId="7" r:id="rId6"/>
     <sheet name="Sheet4" sheetId="8" r:id="rId7"/>
-    <sheet name="References" sheetId="6" r:id="rId8"/>
+    <sheet name="Sheet5" sheetId="9" r:id="rId8"/>
+    <sheet name="References" sheetId="6" r:id="rId9"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="117">
   <si>
     <t>Logarithms can be calculated by division</t>
   </si>
@@ -373,6 +374,21 @@
   </si>
   <si>
     <t>div/1024</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>x2-x+x-1</t>
+  </si>
+  <si>
+    <t>x2=</t>
   </si>
 </sst>
 </file>
@@ -1714,8 +1730,8 @@
       <xdr:rowOff>98901</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="6245257" cy="1016817"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -1760,6 +1776,7 @@
               <a:endParaRPr lang="en-US" sz="1600"/>
             </a:p>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -1882,7 +1899,7 @@
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -1895,7 +1912,7 @@
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -1907,7 +1924,7 @@
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -1919,7 +1936,7 @@
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -1933,7 +1950,7 @@
                                       <a:schemeClr val="tx1"/>
                                     </a:solidFill>
                                     <a:effectLst/>
-                                    <a:latin typeface="+mn-lt"/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:ea typeface="+mn-ea"/>
                                     <a:cs typeface="+mn-cs"/>
                                   </a:rPr>
@@ -1948,7 +1965,7 @@
                                           <a:schemeClr val="tx1"/>
                                         </a:solidFill>
                                         <a:effectLst/>
-                                        <a:latin typeface="+mn-lt"/>
+                                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                         <a:ea typeface="+mn-ea"/>
                                         <a:cs typeface="+mn-cs"/>
                                       </a:rPr>
@@ -1961,7 +1978,7 @@
                                           <a:schemeClr val="tx1"/>
                                         </a:solidFill>
                                         <a:effectLst/>
-                                        <a:latin typeface="+mn-lt"/>
+                                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                         <a:ea typeface="+mn-ea"/>
                                         <a:cs typeface="+mn-cs"/>
                                       </a:rPr>
@@ -1975,7 +1992,7 @@
                                           <a:schemeClr val="tx1"/>
                                         </a:solidFill>
                                         <a:effectLst/>
-                                        <a:latin typeface="+mn-lt"/>
+                                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                         <a:ea typeface="+mn-ea"/>
                                         <a:cs typeface="+mn-cs"/>
                                       </a:rPr>
@@ -1991,7 +2008,7 @@
                                       <a:schemeClr val="tx1"/>
                                     </a:solidFill>
                                     <a:effectLst/>
-                                    <a:latin typeface="+mn-lt"/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:ea typeface="+mn-ea"/>
                                     <a:cs typeface="+mn-cs"/>
                                   </a:rPr>
@@ -2005,7 +2022,7 @@
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -2019,7 +2036,7 @@
                                       <a:schemeClr val="tx1"/>
                                     </a:solidFill>
                                     <a:effectLst/>
-                                    <a:latin typeface="+mn-lt"/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:ea typeface="+mn-ea"/>
                                     <a:cs typeface="+mn-cs"/>
                                   </a:rPr>
@@ -2034,7 +2051,7 @@
                                           <a:schemeClr val="tx1"/>
                                         </a:solidFill>
                                         <a:effectLst/>
-                                        <a:latin typeface="+mn-lt"/>
+                                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                         <a:ea typeface="+mn-ea"/>
                                         <a:cs typeface="+mn-cs"/>
                                       </a:rPr>
@@ -2047,7 +2064,7 @@
                                           <a:schemeClr val="tx1"/>
                                         </a:solidFill>
                                         <a:effectLst/>
-                                        <a:latin typeface="+mn-lt"/>
+                                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                         <a:ea typeface="+mn-ea"/>
                                         <a:cs typeface="+mn-cs"/>
                                       </a:rPr>
@@ -2061,7 +2078,7 @@
                                           <a:schemeClr val="tx1"/>
                                         </a:solidFill>
                                         <a:effectLst/>
-                                        <a:latin typeface="+mn-lt"/>
+                                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                         <a:ea typeface="+mn-ea"/>
                                         <a:cs typeface="+mn-cs"/>
                                       </a:rPr>
@@ -2077,7 +2094,7 @@
                                       <a:schemeClr val="tx1"/>
                                     </a:solidFill>
                                     <a:effectLst/>
-                                    <a:latin typeface="+mn-lt"/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:ea typeface="+mn-ea"/>
                                     <a:cs typeface="+mn-cs"/>
                                   </a:rPr>
@@ -2091,7 +2108,7 @@
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="+mn-lt"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -2105,7 +2122,7 @@
                                       <a:schemeClr val="tx1"/>
                                     </a:solidFill>
                                     <a:effectLst/>
-                                    <a:latin typeface="+mn-lt"/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:ea typeface="+mn-ea"/>
                                     <a:cs typeface="+mn-cs"/>
                                   </a:rPr>
@@ -2120,7 +2137,7 @@
                                           <a:schemeClr val="tx1"/>
                                         </a:solidFill>
                                         <a:effectLst/>
-                                        <a:latin typeface="+mn-lt"/>
+                                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                         <a:ea typeface="+mn-ea"/>
                                         <a:cs typeface="+mn-cs"/>
                                       </a:rPr>
@@ -2133,7 +2150,7 @@
                                           <a:schemeClr val="tx1"/>
                                         </a:solidFill>
                                         <a:effectLst/>
-                                        <a:latin typeface="+mn-lt"/>
+                                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                         <a:ea typeface="+mn-ea"/>
                                         <a:cs typeface="+mn-cs"/>
                                       </a:rPr>
@@ -2147,7 +2164,7 @@
                                           <a:schemeClr val="tx1"/>
                                         </a:solidFill>
                                         <a:effectLst/>
-                                        <a:latin typeface="+mn-lt"/>
+                                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                         <a:ea typeface="+mn-ea"/>
                                         <a:cs typeface="+mn-cs"/>
                                       </a:rPr>
@@ -2163,7 +2180,7 @@
                                       <a:schemeClr val="tx1"/>
                                     </a:solidFill>
                                     <a:effectLst/>
-                                    <a:latin typeface="+mn-lt"/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:ea typeface="+mn-ea"/>
                                     <a:cs typeface="+mn-cs"/>
                                   </a:rPr>
@@ -2192,7 +2209,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -5933,7 +5950,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2C4AA32-FC0E-485A-B3DF-7B3C3B9AAC36}">
   <dimension ref="D4:P18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -6039,6 +6056,78 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A188F2A-3E6A-413F-B5D4-473ED5DEFF88}">
+  <dimension ref="D5:J12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="5" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="J6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>112</v>
+      </c>
+      <c r="E8" t="s">
+        <v>113</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="H8" t="s">
+        <v>112</v>
+      </c>
+      <c r="I8" t="s">
+        <v>114</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="12" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>116</v>
+      </c>
+      <c r="E12">
+        <v>0.405465108108164</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <f>+E12+F12</f>
+        <v>1.4054651081081639</v>
+      </c>
+      <c r="I12">
+        <f>SQRT(G12)</f>
+        <v>1.1855231368928081</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01863960-FF63-4547-8364-6609223CC4B2}">
   <dimension ref="D1:K20"/>
   <sheetViews>

</xml_diff>